<commit_message>
Working on documentation and inline documentation
</commit_message>
<xml_diff>
--- a/documentation/210_Vorlage_GanttDiagramm.110.xlsx
+++ b/documentation/210_Vorlage_GanttDiagramm.110.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="2568"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="12000" windowHeight="2565"/>
   </bookViews>
   <sheets>
     <sheet name="Balkenplan" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="28">
   <si>
     <t>Nr.</t>
   </si>
@@ -38,25 +38,7 @@
     <t>Dauer</t>
   </si>
   <si>
-    <t>❶</t>
-  </si>
-  <si>
-    <t>❸❹❺❻❼❽❾❿</t>
-  </si>
-  <si>
     <t xml:space="preserve">Meilensteine </t>
-  </si>
-  <si>
-    <t>[Vorname 1] SOLL</t>
-  </si>
-  <si>
-    <t>[Vorname 1] IST</t>
-  </si>
-  <si>
-    <t>[Vorname 2] SOLL</t>
-  </si>
-  <si>
-    <t>[Vorname 2] IST</t>
   </si>
   <si>
     <t>Phase</t>
@@ -68,9 +50,6 @@
     <t>Realisation</t>
   </si>
   <si>
-    <t>32h / 24h</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
@@ -78,9 +57,6 @@
   </si>
   <si>
     <t>User Story</t>
-  </si>
-  <si>
-    <t>User Story ...</t>
   </si>
   <si>
     <r>
@@ -135,17 +111,41 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">User Story 1 </t>
+    <t>[Jouni] SOLL</t>
   </si>
   <si>
-    <t xml:space="preserve">User Story 2 </t>
+    <t>[Jouni] IST</t>
+  </si>
+  <si>
+    <t>[Tomaso] SOLL</t>
+  </si>
+  <si>
+    <t>[Tomaso] IST</t>
+  </si>
+  <si>
+    <t>8H</t>
+  </si>
+  <si>
+    <t>Arbeit an Startseite / Edit-Seite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vervollständigung Startseite / Integration Datenbank  </t>
+  </si>
+  <si>
+    <t>Erstellen Tabellen / Verbindung mit View / Session-handling</t>
+  </si>
+  <si>
+    <t>Vervollständigung Verbindung / Beheben von kleineren Fehlern &amp; Bugs</t>
+  </si>
+  <si>
+    <t>2 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +204,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -242,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -377,32 +384,6 @@
       </diagonal>
     </border>
     <border>
-      <left style="thin">
-        <color theme="3" tint="0.39997558519241921"/>
-      </left>
-      <right style="thin">
-        <color theme="3" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="3" tint="0.39997558519241921"/>
-      </left>
-      <right style="thin">
-        <color theme="3" tint="0.39997558519241921"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="3" tint="0.39997558519241921"/>
@@ -434,41 +415,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -481,7 +431,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
@@ -520,12 +470,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -539,12 +483,9 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -555,16 +496,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -574,69 +513,84 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60 % - Akzent1" xfId="2" builtinId="32"/>
@@ -657,7 +611,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -943,69 +897,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK28"/>
+  <dimension ref="A1:BK40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:E26"/>
+      <selection activeCell="AF37" sqref="AF37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.44140625" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.109375" style="5" customWidth="1"/>
-    <col min="8" max="9" width="3.109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="3.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.109375" style="5" customWidth="1"/>
-    <col min="12" max="13" width="3.109375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="3.109375" style="8" customWidth="1"/>
-    <col min="15" max="15" width="3.109375" style="5" customWidth="1"/>
-    <col min="16" max="17" width="3.109375" style="6" customWidth="1"/>
-    <col min="18" max="18" width="3.109375" style="8" customWidth="1"/>
-    <col min="19" max="19" width="3.109375" style="5" customWidth="1"/>
-    <col min="20" max="21" width="3.109375" style="6" customWidth="1"/>
-    <col min="22" max="22" width="3.109375" style="8" customWidth="1"/>
-    <col min="23" max="23" width="3.109375" style="5" customWidth="1"/>
-    <col min="24" max="25" width="3.109375" style="6" customWidth="1"/>
-    <col min="26" max="26" width="3.109375" style="8" customWidth="1"/>
-    <col min="27" max="27" width="3.109375" style="5" customWidth="1"/>
-    <col min="28" max="29" width="3.109375" style="6" customWidth="1"/>
-    <col min="30" max="30" width="3.109375" style="8" customWidth="1"/>
-    <col min="31" max="31" width="3.109375" style="5" customWidth="1"/>
-    <col min="32" max="33" width="3.109375" style="6" customWidth="1"/>
-    <col min="34" max="34" width="3.109375" style="8" customWidth="1"/>
-    <col min="35" max="35" width="3.109375" style="5" customWidth="1"/>
-    <col min="36" max="37" width="3.109375" style="6" customWidth="1"/>
-    <col min="38" max="38" width="3.109375" style="8" customWidth="1"/>
-    <col min="39" max="39" width="3.109375" style="5" customWidth="1"/>
-    <col min="40" max="41" width="3.109375" style="6" customWidth="1"/>
-    <col min="42" max="42" width="3.109375" style="8" customWidth="1"/>
-    <col min="43" max="43" width="3.109375" style="5" customWidth="1"/>
-    <col min="44" max="45" width="3.109375" style="6" customWidth="1"/>
-    <col min="46" max="46" width="3.109375" style="8" customWidth="1"/>
-    <col min="47" max="47" width="3.109375" style="5" customWidth="1"/>
-    <col min="48" max="49" width="3.109375" style="6" customWidth="1"/>
-    <col min="50" max="50" width="3.109375" style="8" customWidth="1"/>
-    <col min="51" max="51" width="3.109375" style="5" customWidth="1"/>
-    <col min="52" max="53" width="3.109375" style="6" customWidth="1"/>
-    <col min="54" max="54" width="3.109375" style="8" customWidth="1"/>
-    <col min="55" max="55" width="3.109375" style="5" customWidth="1"/>
-    <col min="56" max="57" width="3.109375" style="6" customWidth="1"/>
-    <col min="58" max="58" width="3.109375" style="8" customWidth="1"/>
-    <col min="59" max="59" width="3.109375" style="5" customWidth="1"/>
-    <col min="60" max="60" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" style="5" customWidth="1"/>
+    <col min="8" max="9" width="3.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" style="5" customWidth="1"/>
+    <col min="12" max="13" width="3.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="3.140625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="3.140625" style="5" customWidth="1"/>
+    <col min="16" max="17" width="3.140625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="3.140625" style="8" customWidth="1"/>
+    <col min="19" max="19" width="3.140625" style="5" customWidth="1"/>
+    <col min="20" max="21" width="3.140625" style="6" customWidth="1"/>
+    <col min="22" max="22" width="3.140625" style="8" customWidth="1"/>
+    <col min="23" max="23" width="3.140625" style="5" customWidth="1"/>
+    <col min="24" max="25" width="3.140625" style="6" customWidth="1"/>
+    <col min="26" max="26" width="3.140625" style="8" customWidth="1"/>
+    <col min="27" max="27" width="3.140625" style="5" customWidth="1"/>
+    <col min="28" max="29" width="3.140625" style="6" customWidth="1"/>
+    <col min="30" max="30" width="3.140625" style="8" customWidth="1"/>
+    <col min="31" max="31" width="3.140625" style="5" customWidth="1"/>
+    <col min="32" max="33" width="3.140625" style="6" customWidth="1"/>
+    <col min="34" max="34" width="3.140625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="3.140625" style="5" customWidth="1"/>
+    <col min="36" max="37" width="3.140625" style="6" customWidth="1"/>
+    <col min="38" max="38" width="3.140625" style="8" customWidth="1"/>
+    <col min="39" max="39" width="3.140625" style="5" customWidth="1"/>
+    <col min="40" max="41" width="3.140625" style="6" customWidth="1"/>
+    <col min="42" max="42" width="3.140625" style="8" customWidth="1"/>
+    <col min="43" max="43" width="3.140625" style="5" customWidth="1"/>
+    <col min="44" max="45" width="3.140625" style="6" customWidth="1"/>
+    <col min="46" max="46" width="3.140625" style="8" customWidth="1"/>
+    <col min="47" max="47" width="3.140625" style="5" customWidth="1"/>
+    <col min="48" max="49" width="3.140625" style="6" customWidth="1"/>
+    <col min="50" max="50" width="3.140625" style="8" customWidth="1"/>
+    <col min="51" max="51" width="3.140625" style="5" customWidth="1"/>
+    <col min="52" max="53" width="3.140625" style="6" customWidth="1"/>
+    <col min="54" max="54" width="3.140625" style="8" customWidth="1"/>
+    <col min="55" max="55" width="3.140625" style="5" customWidth="1"/>
+    <col min="56" max="57" width="3.140625" style="6" customWidth="1"/>
+    <col min="58" max="58" width="3.140625" style="8" customWidth="1"/>
+    <col min="59" max="59" width="3.140625" style="5" customWidth="1"/>
+    <col min="60" max="60" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="62" width="3.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="19"/>
@@ -1014,95 +968,95 @@
         <v>5</v>
       </c>
       <c r="F1" s="23"/>
-      <c r="G1" s="55">
-        <v>11.1</v>
-      </c>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="55">
-        <v>12.1</v>
-      </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="55">
-        <v>13.1</v>
-      </c>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="56"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="55">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="55">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="55">
+      <c r="G1" s="48">
+        <v>5.04</v>
+      </c>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="48">
+        <v>15.04</v>
+      </c>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="48">
+        <v>16.04</v>
+      </c>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="48">
+        <v>17.04</v>
+      </c>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="48">
+        <v>18.04</v>
+      </c>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="48">
         <v>20.100000000000001</v>
       </c>
-      <c r="AB1" s="56"/>
-      <c r="AC1" s="56"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="55">
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="48">
         <v>25.1</v>
       </c>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="56"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="55">
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="48">
         <v>26.1</v>
       </c>
-      <c r="AJ1" s="56"/>
-      <c r="AK1" s="56"/>
-      <c r="AL1" s="57"/>
-      <c r="AM1" s="55">
+      <c r="AJ1" s="49"/>
+      <c r="AK1" s="49"/>
+      <c r="AL1" s="50"/>
+      <c r="AM1" s="48">
         <v>27.2</v>
       </c>
-      <c r="AN1" s="56"/>
-      <c r="AO1" s="56"/>
-      <c r="AP1" s="57"/>
-      <c r="AQ1" s="55">
+      <c r="AN1" s="49"/>
+      <c r="AO1" s="49"/>
+      <c r="AP1" s="50"/>
+      <c r="AQ1" s="48">
         <v>1.2</v>
       </c>
-      <c r="AR1" s="56"/>
-      <c r="AS1" s="56"/>
-      <c r="AT1" s="57"/>
-      <c r="AU1" s="55">
+      <c r="AR1" s="49"/>
+      <c r="AS1" s="49"/>
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="48">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AV1" s="56"/>
-      <c r="AW1" s="56"/>
-      <c r="AX1" s="57"/>
-      <c r="AY1" s="55">
+      <c r="AV1" s="49"/>
+      <c r="AW1" s="49"/>
+      <c r="AX1" s="50"/>
+      <c r="AY1" s="48">
         <v>3.2</v>
       </c>
-      <c r="AZ1" s="56"/>
-      <c r="BA1" s="56"/>
-      <c r="BB1" s="57"/>
-      <c r="BC1" s="55">
+      <c r="AZ1" s="49"/>
+      <c r="BA1" s="49"/>
+      <c r="BB1" s="50"/>
+      <c r="BC1" s="48">
         <v>8.1999999999999993</v>
       </c>
-      <c r="BD1" s="56"/>
-      <c r="BE1" s="56"/>
-      <c r="BF1" s="57"/>
-      <c r="BG1" s="55">
+      <c r="BD1" s="49"/>
+      <c r="BE1" s="49"/>
+      <c r="BF1" s="50"/>
+      <c r="BG1" s="48">
         <v>9.1999999999999993</v>
       </c>
-      <c r="BH1" s="56"/>
-      <c r="BI1" s="56"/>
-      <c r="BJ1" s="57"/>
-    </row>
-    <row r="2" spans="1:63" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="75"/>
+      <c r="BH1" s="49"/>
+      <c r="BI1" s="49"/>
+      <c r="BJ1" s="50"/>
+    </row>
+    <row r="2" spans="1:63" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="67"/>
       <c r="C2" s="16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>6</v>
@@ -1278,31 +1232,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:63" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="58">
+    <row r="3" spans="1:63" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="68">
         <v>1</v>
       </c>
-      <c r="C3" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="45"/>
+      <c r="C3" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="54"/>
+      <c r="F3" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="42"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="46"/>
+      <c r="K3" s="9"/>
+      <c r="N3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="9"/>
       <c r="V3" s="11"/>
@@ -1327,22 +1279,20 @@
       <c r="BG3" s="9"/>
       <c r="BJ3" s="11"/>
     </row>
-    <row r="4" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="47"/>
+    <row r="4" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="65"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="43"/>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="18"/>
-      <c r="N4" s="48"/>
+      <c r="N4" s="14"/>
       <c r="R4" s="14"/>
       <c r="S4" s="12"/>
       <c r="V4" s="14"/>
@@ -1367,23 +1317,20 @@
       <c r="BG4" s="12"/>
       <c r="BJ4" s="14"/>
     </row>
-    <row r="5" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="50"/>
+    <row r="5" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="65"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="44"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="N5" s="14"/>
       <c r="R5" s="14"/>
       <c r="S5" s="12"/>
       <c r="V5" s="14"/>
@@ -1408,23 +1355,23 @@
       <c r="BG5" s="12"/>
       <c r="BJ5" s="14"/>
     </row>
-    <row r="6" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="71"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="53"/>
+    <row r="6" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="37"/>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
@@ -1474,25 +1421,26 @@
       <c r="BI6" s="13"/>
       <c r="BJ6" s="14"/>
     </row>
-    <row r="7" spans="1:63" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="70" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="58">
+    <row r="7" spans="1:63" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="64" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="68">
         <v>2</v>
       </c>
-      <c r="C7" s="59" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="26" t="s">
-        <v>10</v>
+      <c r="C7" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="54"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="39" t="s">
+        <v>18</v>
       </c>
       <c r="G7" s="9"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="9"/>
-      <c r="N7" s="11"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
       <c r="O7" s="9"/>
       <c r="R7" s="11"/>
       <c r="S7" s="9"/>
@@ -1518,17 +1466,21 @@
       <c r="BG7" s="9"/>
       <c r="BJ7" s="11"/>
     </row>
-    <row r="8" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="37" t="s">
-        <v>11</v>
-      </c>
+    <row r="8" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="65"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12"/>
       <c r="J8" s="14"/>
-      <c r="N8" s="14"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
       <c r="O8" s="12"/>
       <c r="R8" s="14"/>
       <c r="S8" s="12"/>
@@ -1554,17 +1506,21 @@
       <c r="BG8" s="12"/>
       <c r="BJ8" s="14"/>
     </row>
-    <row r="9" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="37" t="s">
-        <v>12</v>
-      </c>
+    <row r="9" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="65"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="12"/>
       <c r="J9" s="14"/>
-      <c r="N9" s="14"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
       <c r="O9" s="12"/>
       <c r="R9" s="14"/>
       <c r="S9" s="12"/>
@@ -1590,23 +1546,23 @@
       <c r="BG9" s="12"/>
       <c r="BJ9" s="14"/>
     </row>
-    <row r="10" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="71"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="14"/>
+    <row r="10" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="65"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
       <c r="O10" s="12"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
@@ -1656,25 +1612,27 @@
       <c r="BI10" s="13"/>
       <c r="BJ10" s="14"/>
     </row>
-    <row r="11" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
-      <c r="B11" s="73">
+    <row r="11" spans="1:63" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="65"/>
+      <c r="B11" s="69">
         <v>3</v>
       </c>
-      <c r="C11" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="26" t="s">
-        <v>10</v>
+      <c r="C11" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="54"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="39" t="s">
+        <v>18</v>
       </c>
       <c r="G11" s="9"/>
       <c r="J11" s="11"/>
       <c r="K11" s="9"/>
       <c r="N11" s="11"/>
-      <c r="O11" s="9"/>
-      <c r="R11" s="11"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
       <c r="S11" s="9"/>
       <c r="V11" s="11"/>
       <c r="W11" s="9"/>
@@ -1699,20 +1657,22 @@
       <c r="BJ11" s="11"/>
       <c r="BK11" s="9"/>
     </row>
-    <row r="12" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="37" t="s">
-        <v>11</v>
+    <row r="12" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="65"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="40" t="s">
+        <v>19</v>
       </c>
       <c r="G12" s="12"/>
       <c r="J12" s="14"/>
       <c r="N12" s="14"/>
-      <c r="O12" s="12"/>
-      <c r="R12" s="14"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
       <c r="S12" s="12"/>
       <c r="V12" s="14"/>
       <c r="W12" s="12"/>
@@ -1737,20 +1697,21 @@
       <c r="BJ12" s="14"/>
       <c r="BK12" s="12"/>
     </row>
-    <row r="13" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="71"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="37" t="s">
-        <v>12</v>
+    <row r="13" spans="1:63" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="65"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="40" t="s">
+        <v>20</v>
       </c>
       <c r="G13" s="12"/>
       <c r="J13" s="14"/>
       <c r="N13" s="14"/>
-      <c r="O13" s="12"/>
-      <c r="R13" s="14"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
       <c r="S13" s="12"/>
       <c r="V13" s="14"/>
       <c r="W13" s="12"/>
@@ -1775,73 +1736,74 @@
       <c r="BJ13" s="14"/>
       <c r="BK13" s="12"/>
     </row>
-    <row r="14" spans="1:63" s="39" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="71"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="38"/>
-      <c r="J14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="38"/>
-      <c r="R14" s="40"/>
-      <c r="S14" s="38"/>
-      <c r="V14" s="40"/>
-      <c r="W14" s="38"/>
-      <c r="Z14" s="40"/>
-      <c r="AA14" s="38"/>
-      <c r="AD14" s="40"/>
-      <c r="AE14" s="38"/>
-      <c r="AH14" s="40"/>
-      <c r="AI14" s="38"/>
-      <c r="AL14" s="40"/>
-      <c r="AM14" s="38"/>
-      <c r="AP14" s="40"/>
-      <c r="AQ14" s="38"/>
-      <c r="AT14" s="40"/>
-      <c r="AU14" s="38"/>
-      <c r="AX14" s="40"/>
-      <c r="AY14" s="38"/>
-      <c r="BB14" s="40"/>
-      <c r="BC14" s="38"/>
-      <c r="BF14" s="40"/>
-      <c r="BG14" s="38"/>
-      <c r="BJ14" s="40"/>
-      <c r="BK14" s="38"/>
-    </row>
-    <row r="15" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
-      <c r="B15" s="58">
+    <row r="14" spans="1:63" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="65"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="35"/>
+      <c r="J14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46"/>
+      <c r="S14" s="35"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="35"/>
+      <c r="Z14" s="37"/>
+      <c r="AA14" s="35"/>
+      <c r="AD14" s="37"/>
+      <c r="AE14" s="35"/>
+      <c r="AH14" s="37"/>
+      <c r="AI14" s="35"/>
+      <c r="AL14" s="37"/>
+      <c r="AM14" s="35"/>
+      <c r="AP14" s="37"/>
+      <c r="AQ14" s="35"/>
+      <c r="AT14" s="37"/>
+      <c r="AU14" s="35"/>
+      <c r="AX14" s="37"/>
+      <c r="AY14" s="35"/>
+      <c r="BB14" s="37"/>
+      <c r="BC14" s="35"/>
+      <c r="BF14" s="37"/>
+      <c r="BG14" s="35"/>
+      <c r="BJ14" s="37"/>
+      <c r="BK14" s="35"/>
+    </row>
+    <row r="15" spans="1:63" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="65"/>
+      <c r="B15" s="71">
         <v>4</v>
       </c>
-      <c r="C15" s="59" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="62"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="14"/>
+      <c r="C15" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="11"/>
       <c r="O15" s="12"/>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="14"/>
-      <c r="S15" s="12"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="14"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
       <c r="W15" s="12"/>
       <c r="X15" s="13"/>
       <c r="Y15" s="13"/>
@@ -1883,16 +1845,16 @@
       <c r="BI15" s="13"/>
       <c r="BJ15" s="14"/>
     </row>
-    <row r="16" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="13"/>
+    <row r="16" spans="1:63" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="65"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="12"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
       <c r="J16" s="14"/>
@@ -1904,10 +1866,10 @@
       <c r="P16" s="13"/>
       <c r="Q16" s="13"/>
       <c r="R16" s="14"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="14"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="18"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
       <c r="W16" s="12"/>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -1949,16 +1911,16 @@
       <c r="BI16" s="13"/>
       <c r="BJ16" s="14"/>
     </row>
-    <row r="17" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="71"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="13"/>
+    <row r="17" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="65"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="12"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="14"/>
@@ -1970,10 +1932,10 @@
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="14"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="14"/>
+      <c r="S17" s="44"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="13"/>
       <c r="W17" s="12"/>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -2015,31 +1977,31 @@
       <c r="BI17" s="13"/>
       <c r="BJ17" s="14"/>
     </row>
-    <row r="18" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="72"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="14"/>
+    <row r="18" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="65"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="37"/>
       <c r="O18" s="12"/>
       <c r="P18" s="13"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="14"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="14"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="46"/>
+      <c r="U18" s="46"/>
+      <c r="V18" s="46"/>
       <c r="W18" s="12"/>
       <c r="X18" s="13"/>
       <c r="Y18" s="13"/>
@@ -2081,154 +2043,232 @@
       <c r="BI18" s="13"/>
       <c r="BJ18" s="14"/>
     </row>
-    <row r="19" spans="1:62" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="70" t="s">
+    <row r="19" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="65"/>
+      <c r="C19" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="54"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="58">
-        <v>5</v>
-      </c>
-      <c r="C19" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="26" t="s">
-        <v>10</v>
-      </c>
       <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
       <c r="J19" s="11"/>
       <c r="K19" s="9"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
       <c r="N19" s="11"/>
-      <c r="O19" s="9"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
       <c r="R19" s="11"/>
       <c r="S19" s="9"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="9"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
       <c r="Z19" s="11"/>
       <c r="AA19" s="9"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
       <c r="AD19" s="11"/>
       <c r="AE19" s="9"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
       <c r="AH19" s="11"/>
       <c r="AI19" s="9"/>
+      <c r="AJ19" s="10"/>
+      <c r="AK19" s="10"/>
       <c r="AL19" s="11"/>
       <c r="AM19" s="9"/>
+      <c r="AN19" s="10"/>
+      <c r="AO19" s="10"/>
       <c r="AP19" s="11"/>
       <c r="AQ19" s="9"/>
+      <c r="AR19" s="10"/>
+      <c r="AS19" s="10"/>
       <c r="AT19" s="11"/>
       <c r="AU19" s="9"/>
+      <c r="AV19" s="10"/>
+      <c r="AW19" s="10"/>
       <c r="AX19" s="11"/>
       <c r="AY19" s="9"/>
+      <c r="AZ19" s="10"/>
+      <c r="BA19" s="10"/>
       <c r="BB19" s="11"/>
       <c r="BC19" s="9"/>
+      <c r="BD19" s="10"/>
+      <c r="BE19" s="10"/>
       <c r="BF19" s="11"/>
       <c r="BG19" s="9"/>
+      <c r="BH19" s="10"/>
+      <c r="BI19" s="10"/>
       <c r="BJ19" s="11"/>
     </row>
-    <row r="20" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="71"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="37" t="s">
-        <v>11</v>
-      </c>
+    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A20" s="65"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="12"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
       <c r="J20" s="14"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
       <c r="N20" s="14"/>
-      <c r="O20" s="12"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
       <c r="R20" s="14"/>
       <c r="S20" s="12"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="12"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="43"/>
+      <c r="W20" s="18"/>
+      <c r="X20" s="18"/>
+      <c r="Y20" s="13"/>
       <c r="Z20" s="14"/>
-      <c r="AA20" s="12"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13"/>
+      <c r="AC20" s="13"/>
       <c r="AD20" s="14"/>
       <c r="AE20" s="12"/>
+      <c r="AF20" s="13"/>
+      <c r="AG20" s="13"/>
       <c r="AH20" s="14"/>
       <c r="AI20" s="12"/>
+      <c r="AJ20" s="13"/>
+      <c r="AK20" s="13"/>
       <c r="AL20" s="14"/>
       <c r="AM20" s="12"/>
+      <c r="AN20" s="13"/>
+      <c r="AO20" s="13"/>
       <c r="AP20" s="14"/>
       <c r="AQ20" s="12"/>
+      <c r="AR20" s="13"/>
+      <c r="AS20" s="13"/>
       <c r="AT20" s="14"/>
       <c r="AU20" s="12"/>
+      <c r="AV20" s="13"/>
+      <c r="AW20" s="13"/>
       <c r="AX20" s="14"/>
       <c r="AY20" s="12"/>
+      <c r="AZ20" s="13"/>
+      <c r="BA20" s="13"/>
       <c r="BB20" s="14"/>
       <c r="BC20" s="12"/>
+      <c r="BD20" s="13"/>
+      <c r="BE20" s="13"/>
       <c r="BF20" s="14"/>
       <c r="BG20" s="12"/>
+      <c r="BH20" s="13"/>
+      <c r="BI20" s="13"/>
       <c r="BJ20" s="14"/>
     </row>
-    <row r="21" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="71"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="37" t="s">
-        <v>12</v>
-      </c>
+    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A21" s="65"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="14"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
       <c r="N21" s="14"/>
-      <c r="O21" s="12"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
       <c r="R21" s="14"/>
       <c r="S21" s="12"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="12"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
       <c r="Z21" s="14"/>
       <c r="AA21" s="12"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13"/>
       <c r="AD21" s="14"/>
       <c r="AE21" s="12"/>
+      <c r="AF21" s="13"/>
+      <c r="AG21" s="13"/>
       <c r="AH21" s="14"/>
       <c r="AI21" s="12"/>
+      <c r="AJ21" s="13"/>
+      <c r="AK21" s="13"/>
       <c r="AL21" s="14"/>
       <c r="AM21" s="12"/>
+      <c r="AN21" s="13"/>
+      <c r="AO21" s="13"/>
       <c r="AP21" s="14"/>
       <c r="AQ21" s="12"/>
+      <c r="AR21" s="13"/>
+      <c r="AS21" s="13"/>
       <c r="AT21" s="14"/>
       <c r="AU21" s="12"/>
+      <c r="AV21" s="13"/>
+      <c r="AW21" s="13"/>
       <c r="AX21" s="14"/>
       <c r="AY21" s="12"/>
+      <c r="AZ21" s="13"/>
+      <c r="BA21" s="13"/>
       <c r="BB21" s="14"/>
       <c r="BC21" s="12"/>
+      <c r="BD21" s="13"/>
+      <c r="BE21" s="13"/>
       <c r="BF21" s="14"/>
       <c r="BG21" s="12"/>
+      <c r="BH21" s="13"/>
+      <c r="BI21" s="13"/>
       <c r="BJ21" s="14"/>
     </row>
-    <row r="22" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="72"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="12"/>
+    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A22" s="65"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="13"/>
       <c r="Q22" s="13"/>
       <c r="R22" s="14"/>
       <c r="S22" s="12"/>
       <c r="T22" s="13"/>
       <c r="U22" s="13"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="46"/>
+      <c r="X22" s="46"/>
+      <c r="Y22" s="36"/>
       <c r="Z22" s="14"/>
-      <c r="AA22" s="12"/>
+      <c r="AA22" s="13"/>
       <c r="AB22" s="13"/>
       <c r="AC22" s="13"/>
       <c r="AD22" s="14"/>
@@ -2265,137 +2305,209 @@
       <c r="BI22" s="13"/>
       <c r="BJ22" s="14"/>
     </row>
-    <row r="23" spans="1:62" s="10" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="58">
-        <v>6</v>
-      </c>
-      <c r="C23" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="26" t="s">
-        <v>10</v>
-      </c>
+    <row r="23" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="65"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
       <c r="J23" s="11"/>
       <c r="K23" s="9"/>
-      <c r="O23" s="45"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
       <c r="R23" s="11"/>
-      <c r="S23" s="45"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
       <c r="V23" s="11"/>
       <c r="W23" s="9"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
       <c r="Z23" s="11"/>
-      <c r="AA23" s="45"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10"/>
       <c r="AD23" s="11"/>
       <c r="AE23" s="9"/>
+      <c r="AF23" s="10"/>
+      <c r="AG23" s="10"/>
       <c r="AH23" s="11"/>
       <c r="AI23" s="9"/>
+      <c r="AJ23" s="10"/>
+      <c r="AK23" s="10"/>
       <c r="AL23" s="11"/>
       <c r="AM23" s="9"/>
+      <c r="AN23" s="10"/>
+      <c r="AO23" s="10"/>
       <c r="AP23" s="11"/>
       <c r="AQ23" s="9"/>
+      <c r="AR23" s="10"/>
+      <c r="AS23" s="10"/>
       <c r="AT23" s="11"/>
       <c r="AU23" s="9"/>
+      <c r="AV23" s="10"/>
+      <c r="AW23" s="10"/>
       <c r="AX23" s="11"/>
       <c r="AY23" s="9"/>
+      <c r="AZ23" s="10"/>
+      <c r="BA23" s="10"/>
       <c r="BB23" s="11"/>
       <c r="BC23" s="9"/>
+      <c r="BD23" s="10"/>
+      <c r="BE23" s="10"/>
       <c r="BF23" s="11"/>
       <c r="BG23" s="9"/>
+      <c r="BH23" s="10"/>
+      <c r="BI23" s="10"/>
       <c r="BJ23" s="11"/>
     </row>
-    <row r="24" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="71"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="37" t="s">
-        <v>11</v>
-      </c>
+    <row r="24" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="65"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
       <c r="J24" s="14"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
       <c r="N24" s="14"/>
       <c r="O24" s="12"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
       <c r="R24" s="14"/>
       <c r="S24" s="12"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
       <c r="V24" s="14"/>
       <c r="W24" s="12"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
       <c r="Z24" s="14"/>
       <c r="AA24" s="12"/>
+      <c r="AB24" s="13"/>
+      <c r="AC24" s="13"/>
       <c r="AD24" s="14"/>
       <c r="AE24" s="12"/>
+      <c r="AF24" s="13"/>
+      <c r="AG24" s="13"/>
       <c r="AH24" s="14"/>
       <c r="AI24" s="12"/>
+      <c r="AJ24" s="13"/>
+      <c r="AK24" s="13"/>
       <c r="AL24" s="14"/>
       <c r="AM24" s="12"/>
+      <c r="AN24" s="13"/>
+      <c r="AO24" s="13"/>
       <c r="AP24" s="14"/>
       <c r="AQ24" s="12"/>
+      <c r="AR24" s="13"/>
+      <c r="AS24" s="13"/>
       <c r="AT24" s="14"/>
       <c r="AU24" s="12"/>
+      <c r="AV24" s="13"/>
+      <c r="AW24" s="13"/>
       <c r="AX24" s="14"/>
       <c r="AY24" s="12"/>
+      <c r="AZ24" s="13"/>
+      <c r="BA24" s="13"/>
       <c r="BB24" s="14"/>
       <c r="BC24" s="12"/>
+      <c r="BD24" s="13"/>
+      <c r="BE24" s="13"/>
       <c r="BF24" s="14"/>
       <c r="BG24" s="12"/>
+      <c r="BH24" s="13"/>
+      <c r="BI24" s="13"/>
       <c r="BJ24" s="14"/>
     </row>
-    <row r="25" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="71"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="37" t="s">
-        <v>12</v>
-      </c>
+    <row r="25" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="65"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
       <c r="J25" s="14"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
       <c r="N25" s="14"/>
       <c r="O25" s="12"/>
-      <c r="S25" s="49"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
       <c r="V25" s="14"/>
-      <c r="W25" s="49"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="12"/>
+      <c r="AB25" s="13"/>
+      <c r="AC25" s="13"/>
       <c r="AD25" s="14"/>
       <c r="AE25" s="12"/>
+      <c r="AF25" s="13"/>
+      <c r="AG25" s="13"/>
       <c r="AH25" s="14"/>
       <c r="AI25" s="12"/>
+      <c r="AJ25" s="13"/>
+      <c r="AK25" s="13"/>
       <c r="AL25" s="14"/>
       <c r="AM25" s="12"/>
+      <c r="AN25" s="13"/>
+      <c r="AO25" s="13"/>
       <c r="AP25" s="14"/>
       <c r="AQ25" s="12"/>
+      <c r="AR25" s="13"/>
+      <c r="AS25" s="13"/>
       <c r="AT25" s="14"/>
       <c r="AU25" s="12"/>
+      <c r="AV25" s="13"/>
+      <c r="AW25" s="13"/>
       <c r="AX25" s="14"/>
       <c r="AY25" s="12"/>
+      <c r="AZ25" s="13"/>
+      <c r="BA25" s="13"/>
       <c r="BB25" s="14"/>
       <c r="BC25" s="12"/>
+      <c r="BD25" s="13"/>
+      <c r="BE25" s="13"/>
       <c r="BF25" s="14"/>
       <c r="BG25" s="12"/>
+      <c r="BH25" s="13"/>
+      <c r="BI25" s="13"/>
       <c r="BJ25" s="14"/>
     </row>
-    <row r="26" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="72"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="14"/>
+    <row r="26" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="65"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="37"/>
       <c r="O26" s="12"/>
       <c r="P26" s="13"/>
       <c r="Q26" s="13"/>
@@ -2445,145 +2557,827 @@
       <c r="BI26" s="13"/>
       <c r="BJ26" s="14"/>
     </row>
-    <row r="27" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="68"/>
-      <c r="B27" s="76">
+    <row r="27" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="65"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="11"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="11"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="10"/>
+      <c r="AH27" s="11"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="10"/>
+      <c r="AK27" s="10"/>
+      <c r="AL27" s="11"/>
+      <c r="AM27" s="9"/>
+      <c r="AN27" s="10"/>
+      <c r="AO27" s="10"/>
+      <c r="AP27" s="11"/>
+      <c r="AQ27" s="9"/>
+      <c r="AR27" s="10"/>
+      <c r="AS27" s="10"/>
+      <c r="AT27" s="11"/>
+      <c r="AU27" s="9"/>
+      <c r="AV27" s="10"/>
+      <c r="AW27" s="10"/>
+      <c r="AX27" s="11"/>
+      <c r="AY27" s="9"/>
+      <c r="AZ27" s="10"/>
+      <c r="BA27" s="10"/>
+      <c r="BB27" s="11"/>
+      <c r="BC27" s="9"/>
+      <c r="BD27" s="10"/>
+      <c r="BE27" s="10"/>
+      <c r="BF27" s="11"/>
+      <c r="BG27" s="9"/>
+      <c r="BH27" s="10"/>
+      <c r="BI27" s="10"/>
+      <c r="BJ27" s="11"/>
+    </row>
+    <row r="28" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="65"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="14"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="12"/>
+      <c r="AB28" s="13"/>
+      <c r="AC28" s="13"/>
+      <c r="AD28" s="14"/>
+      <c r="AE28" s="12"/>
+      <c r="AF28" s="13"/>
+      <c r="AG28" s="13"/>
+      <c r="AH28" s="14"/>
+      <c r="AI28" s="12"/>
+      <c r="AJ28" s="13"/>
+      <c r="AK28" s="13"/>
+      <c r="AL28" s="14"/>
+      <c r="AM28" s="12"/>
+      <c r="AN28" s="13"/>
+      <c r="AO28" s="13"/>
+      <c r="AP28" s="14"/>
+      <c r="AQ28" s="12"/>
+      <c r="AR28" s="13"/>
+      <c r="AS28" s="13"/>
+      <c r="AT28" s="14"/>
+      <c r="AU28" s="12"/>
+      <c r="AV28" s="13"/>
+      <c r="AW28" s="13"/>
+      <c r="AX28" s="14"/>
+      <c r="AY28" s="12"/>
+      <c r="AZ28" s="13"/>
+      <c r="BA28" s="13"/>
+      <c r="BB28" s="14"/>
+      <c r="BC28" s="12"/>
+      <c r="BD28" s="13"/>
+      <c r="BE28" s="13"/>
+      <c r="BF28" s="14"/>
+      <c r="BG28" s="12"/>
+      <c r="BH28" s="13"/>
+      <c r="BI28" s="13"/>
+      <c r="BJ28" s="14"/>
+    </row>
+    <row r="29" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="65"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="14"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
+      <c r="V29" s="14"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="14"/>
+      <c r="AA29" s="12"/>
+      <c r="AB29" s="13"/>
+      <c r="AC29" s="13"/>
+      <c r="AD29" s="14"/>
+      <c r="AE29" s="12"/>
+      <c r="AF29" s="13"/>
+      <c r="AG29" s="13"/>
+      <c r="AH29" s="14"/>
+      <c r="AI29" s="12"/>
+      <c r="AJ29" s="13"/>
+      <c r="AK29" s="13"/>
+      <c r="AL29" s="14"/>
+      <c r="AM29" s="12"/>
+      <c r="AN29" s="13"/>
+      <c r="AO29" s="13"/>
+      <c r="AP29" s="14"/>
+      <c r="AQ29" s="12"/>
+      <c r="AR29" s="13"/>
+      <c r="AS29" s="13"/>
+      <c r="AT29" s="14"/>
+      <c r="AU29" s="12"/>
+      <c r="AV29" s="13"/>
+      <c r="AW29" s="13"/>
+      <c r="AX29" s="14"/>
+      <c r="AY29" s="12"/>
+      <c r="AZ29" s="13"/>
+      <c r="BA29" s="13"/>
+      <c r="BB29" s="14"/>
+      <c r="BC29" s="12"/>
+      <c r="BD29" s="13"/>
+      <c r="BE29" s="13"/>
+      <c r="BF29" s="14"/>
+      <c r="BG29" s="12"/>
+      <c r="BH29" s="13"/>
+      <c r="BI29" s="13"/>
+      <c r="BJ29" s="14"/>
+    </row>
+    <row r="30" spans="1:62" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="66"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="37"/>
+      <c r="O30" s="35"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="35"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="36"/>
+      <c r="V30" s="37"/>
+      <c r="W30" s="35"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="37"/>
+      <c r="AA30" s="35"/>
+      <c r="AB30" s="36"/>
+      <c r="AC30" s="36"/>
+      <c r="AD30" s="37"/>
+      <c r="AE30" s="35"/>
+      <c r="AF30" s="36"/>
+      <c r="AG30" s="36"/>
+      <c r="AH30" s="37"/>
+      <c r="AI30" s="35"/>
+      <c r="AJ30" s="36"/>
+      <c r="AK30" s="36"/>
+      <c r="AL30" s="37"/>
+      <c r="AM30" s="35"/>
+      <c r="AN30" s="36"/>
+      <c r="AO30" s="36"/>
+      <c r="AP30" s="37"/>
+      <c r="AQ30" s="35"/>
+      <c r="AR30" s="36"/>
+      <c r="AS30" s="36"/>
+      <c r="AT30" s="37"/>
+      <c r="AU30" s="35"/>
+      <c r="AV30" s="36"/>
+      <c r="AW30" s="36"/>
+      <c r="AX30" s="37"/>
+      <c r="AY30" s="35"/>
+      <c r="AZ30" s="36"/>
+      <c r="BA30" s="36"/>
+      <c r="BB30" s="37"/>
+      <c r="BC30" s="35"/>
+      <c r="BD30" s="36"/>
+      <c r="BE30" s="36"/>
+      <c r="BF30" s="37"/>
+      <c r="BG30" s="35"/>
+      <c r="BH30" s="36"/>
+      <c r="BI30" s="36"/>
+      <c r="BJ30" s="37"/>
+    </row>
+    <row r="31" spans="1:62" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="68" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="77"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="30"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="29"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="36" t="s">
+      <c r="B31" s="68">
+        <v>5</v>
+      </c>
+      <c r="C31" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="57"/>
+      <c r="F31" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="17"/>
+      <c r="N31" s="78"/>
+      <c r="O31" s="77"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="9"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="9"/>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="9"/>
+      <c r="AH31" s="11"/>
+      <c r="AI31" s="9"/>
+      <c r="AL31" s="11"/>
+      <c r="AM31" s="9"/>
+      <c r="AP31" s="11"/>
+      <c r="AQ31" s="9"/>
+      <c r="AT31" s="11"/>
+      <c r="AU31" s="9"/>
+      <c r="AX31" s="11"/>
+      <c r="AY31" s="9"/>
+      <c r="BB31" s="11"/>
+      <c r="BC31" s="9"/>
+      <c r="BF31" s="11"/>
+      <c r="BG31" s="9"/>
+      <c r="BJ31" s="11"/>
+    </row>
+    <row r="32" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="65"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="12"/>
+      <c r="H32" s="74"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="74"/>
+      <c r="L32" s="74"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="75"/>
+      <c r="Q32" s="74"/>
+      <c r="R32" s="14"/>
+      <c r="S32" s="12"/>
+      <c r="U32" s="74"/>
+      <c r="V32" s="14"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="74"/>
+      <c r="Y32" s="74"/>
+      <c r="Z32" s="76"/>
+      <c r="AA32" s="12"/>
+      <c r="AD32" s="14"/>
+      <c r="AE32" s="12"/>
+      <c r="AH32" s="14"/>
+      <c r="AI32" s="12"/>
+      <c r="AL32" s="14"/>
+      <c r="AM32" s="12"/>
+      <c r="AP32" s="14"/>
+      <c r="AQ32" s="12"/>
+      <c r="AT32" s="14"/>
+      <c r="AU32" s="12"/>
+      <c r="AX32" s="14"/>
+      <c r="AY32" s="12"/>
+      <c r="BB32" s="14"/>
+      <c r="BC32" s="12"/>
+      <c r="BF32" s="14"/>
+      <c r="BG32" s="12"/>
+      <c r="BJ32" s="14"/>
+    </row>
+    <row r="33" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="65"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="12"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="79"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="38"/>
+      <c r="R33" s="79"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="38"/>
+      <c r="U33" s="38"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="80"/>
+      <c r="X33" s="38"/>
+      <c r="Y33" s="38"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="12"/>
+      <c r="AD33" s="14"/>
+      <c r="AE33" s="12"/>
+      <c r="AH33" s="14"/>
+      <c r="AI33" s="12"/>
+      <c r="AL33" s="14"/>
+      <c r="AM33" s="12"/>
+      <c r="AP33" s="14"/>
+      <c r="AQ33" s="12"/>
+      <c r="AT33" s="14"/>
+      <c r="AU33" s="12"/>
+      <c r="AX33" s="14"/>
+      <c r="AY33" s="12"/>
+      <c r="BB33" s="14"/>
+      <c r="BC33" s="12"/>
+      <c r="BF33" s="14"/>
+      <c r="BG33" s="12"/>
+      <c r="BJ33" s="14"/>
+    </row>
+    <row r="34" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="66"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="35"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="74"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="74"/>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="74"/>
+      <c r="U34" s="74"/>
+      <c r="V34" s="76"/>
+      <c r="W34" s="75"/>
+      <c r="X34" s="74"/>
+      <c r="Y34" s="74"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="13"/>
+      <c r="AC34" s="13"/>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="12"/>
+      <c r="AF34" s="13"/>
+      <c r="AG34" s="13"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="12"/>
+      <c r="AJ34" s="13"/>
+      <c r="AK34" s="13"/>
+      <c r="AL34" s="14"/>
+      <c r="AM34" s="12"/>
+      <c r="AN34" s="13"/>
+      <c r="AO34" s="13"/>
+      <c r="AP34" s="14"/>
+      <c r="AQ34" s="12"/>
+      <c r="AR34" s="13"/>
+      <c r="AS34" s="13"/>
+      <c r="AT34" s="14"/>
+      <c r="AU34" s="12"/>
+      <c r="AV34" s="13"/>
+      <c r="AW34" s="13"/>
+      <c r="AX34" s="14"/>
+      <c r="AY34" s="12"/>
+      <c r="AZ34" s="13"/>
+      <c r="BA34" s="13"/>
+      <c r="BB34" s="14"/>
+      <c r="BC34" s="12"/>
+      <c r="BD34" s="13"/>
+      <c r="BE34" s="13"/>
+      <c r="BF34" s="14"/>
+      <c r="BG34" s="12"/>
+      <c r="BH34" s="13"/>
+      <c r="BI34" s="13"/>
+      <c r="BJ34" s="14"/>
+    </row>
+    <row r="35" spans="1:62" s="10" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="68">
+        <v>6</v>
+      </c>
+      <c r="C35" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="54"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="77"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="9"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="72"/>
+      <c r="R35" s="78"/>
+      <c r="S35" s="72"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="78"/>
+      <c r="W35" s="77"/>
+      <c r="X35" s="17"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="9"/>
+      <c r="AD35" s="11"/>
+      <c r="AE35" s="9"/>
+      <c r="AH35" s="11"/>
+      <c r="AI35" s="9"/>
+      <c r="AL35" s="11"/>
+      <c r="AM35" s="9"/>
+      <c r="AP35" s="11"/>
+      <c r="AQ35" s="9"/>
+      <c r="AT35" s="11"/>
+      <c r="AU35" s="9"/>
+      <c r="AX35" s="11"/>
+      <c r="AY35" s="9"/>
+      <c r="BB35" s="11"/>
+      <c r="BC35" s="9"/>
+      <c r="BF35" s="11"/>
+      <c r="BG35" s="9"/>
+      <c r="BJ35" s="11"/>
+    </row>
+    <row r="36" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="65"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="83"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="84"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="12"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="12"/>
+      <c r="V36" s="84"/>
+      <c r="W36" s="83"/>
+      <c r="X36" s="18"/>
+      <c r="Y36" s="18"/>
+      <c r="Z36" s="84"/>
+      <c r="AA36" s="12"/>
+      <c r="AD36" s="14"/>
+      <c r="AE36" s="12"/>
+      <c r="AH36" s="14"/>
+      <c r="AI36" s="12"/>
+      <c r="AL36" s="14"/>
+      <c r="AM36" s="12"/>
+      <c r="AP36" s="14"/>
+      <c r="AQ36" s="12"/>
+      <c r="AT36" s="14"/>
+      <c r="AU36" s="12"/>
+      <c r="AX36" s="14"/>
+      <c r="AY36" s="12"/>
+      <c r="BB36" s="14"/>
+      <c r="BC36" s="12"/>
+      <c r="BF36" s="14"/>
+      <c r="BG36" s="12"/>
+      <c r="BJ36" s="14"/>
+    </row>
+    <row r="37" spans="1:62" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="65"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="80"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="14"/>
+      <c r="N37" s="79"/>
+      <c r="O37" s="12"/>
+      <c r="R37" s="38"/>
+      <c r="S37" s="73"/>
+      <c r="V37" s="79"/>
+      <c r="W37" s="80"/>
+      <c r="X37" s="38"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="12"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="12"/>
+      <c r="AH37" s="14"/>
+      <c r="AI37" s="12"/>
+      <c r="AL37" s="14"/>
+      <c r="AM37" s="12"/>
+      <c r="AP37" s="14"/>
+      <c r="AQ37" s="12"/>
+      <c r="AT37" s="14"/>
+      <c r="AU37" s="12"/>
+      <c r="AX37" s="14"/>
+      <c r="AY37" s="12"/>
+      <c r="BB37" s="14"/>
+      <c r="BC37" s="12"/>
+      <c r="BF37" s="14"/>
+      <c r="BG37" s="12"/>
+      <c r="BJ37" s="14"/>
+    </row>
+    <row r="38" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="66"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="85"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="86"/>
+      <c r="K38" s="13"/>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="12"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="84"/>
+      <c r="W38" s="83"/>
+      <c r="X38" s="18"/>
+      <c r="Y38" s="18"/>
+      <c r="Z38" s="84"/>
+      <c r="AA38" s="12"/>
+      <c r="AB38" s="13"/>
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="14"/>
+      <c r="AE38" s="12"/>
+      <c r="AF38" s="13"/>
+      <c r="AG38" s="13"/>
+      <c r="AH38" s="14"/>
+      <c r="AI38" s="12"/>
+      <c r="AJ38" s="13"/>
+      <c r="AK38" s="13"/>
+      <c r="AL38" s="14"/>
+      <c r="AM38" s="12"/>
+      <c r="AN38" s="13"/>
+      <c r="AO38" s="13"/>
+      <c r="AP38" s="14"/>
+      <c r="AQ38" s="12"/>
+      <c r="AR38" s="13"/>
+      <c r="AS38" s="13"/>
+      <c r="AT38" s="14"/>
+      <c r="AU38" s="12"/>
+      <c r="AV38" s="13"/>
+      <c r="AW38" s="13"/>
+      <c r="AX38" s="14"/>
+      <c r="AY38" s="12"/>
+      <c r="AZ38" s="13"/>
+      <c r="BA38" s="13"/>
+      <c r="BB38" s="14"/>
+      <c r="BC38" s="12"/>
+      <c r="BD38" s="13"/>
+      <c r="BE38" s="13"/>
+      <c r="BF38" s="14"/>
+      <c r="BG38" s="12"/>
+      <c r="BH38" s="13"/>
+      <c r="BI38" s="13"/>
+      <c r="BJ38" s="14"/>
+    </row>
+    <row r="39" spans="1:62" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="60"/>
+      <c r="B39" s="47">
+        <v>11</v>
+      </c>
+      <c r="C39" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="S27" s="29"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="29"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="31"/>
-      <c r="AA27" s="29"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
-      <c r="AD27" s="31"/>
-      <c r="AE27" s="29"/>
-      <c r="AF27" s="30"/>
-      <c r="AG27" s="30"/>
-      <c r="AH27" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI27" s="29"/>
-      <c r="AJ27" s="30"/>
-      <c r="AK27" s="30"/>
-      <c r="AL27" s="31"/>
-      <c r="AM27" s="29"/>
-      <c r="AN27" s="30"/>
-      <c r="AO27" s="30"/>
-      <c r="AP27" s="31"/>
-      <c r="AQ27" s="29"/>
-      <c r="AR27" s="30"/>
-      <c r="AS27" s="30"/>
-      <c r="AT27" s="31"/>
-      <c r="AU27" s="29"/>
-      <c r="AV27" s="30"/>
-      <c r="AW27" s="30"/>
-      <c r="AX27" s="31"/>
-      <c r="AY27" s="29"/>
-      <c r="AZ27" s="30"/>
-      <c r="BA27" s="30"/>
-      <c r="BB27" s="31"/>
-      <c r="BC27" s="29"/>
-      <c r="BD27" s="30"/>
-      <c r="BE27" s="30"/>
-      <c r="BF27" s="31"/>
-      <c r="BG27" s="29"/>
-      <c r="BH27" s="30"/>
-      <c r="BI27" s="30"/>
-      <c r="BJ27" s="31"/>
-    </row>
-    <row r="28" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="69"/>
-      <c r="B28" s="76"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="33"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="34"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="34"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="35"/>
-      <c r="AA28" s="33"/>
-      <c r="AB28" s="34"/>
-      <c r="AC28" s="34"/>
-      <c r="AD28" s="35"/>
-      <c r="AE28" s="33"/>
-      <c r="AF28" s="34"/>
-      <c r="AG28" s="34"/>
-      <c r="AH28" s="35"/>
-      <c r="AI28" s="33"/>
-      <c r="AJ28" s="34"/>
-      <c r="AK28" s="34"/>
-      <c r="AL28" s="35"/>
-      <c r="AM28" s="33"/>
-      <c r="AN28" s="34"/>
-      <c r="AO28" s="34"/>
-      <c r="AP28" s="35"/>
-      <c r="AQ28" s="33"/>
-      <c r="AR28" s="34"/>
-      <c r="AS28" s="34"/>
-      <c r="AT28" s="35"/>
-      <c r="AU28" s="33"/>
-      <c r="AV28" s="34"/>
-      <c r="AW28" s="34"/>
-      <c r="AX28" s="35"/>
-      <c r="AY28" s="33"/>
-      <c r="AZ28" s="34"/>
-      <c r="BA28" s="34"/>
-      <c r="BB28" s="35"/>
-      <c r="BC28" s="33"/>
-      <c r="BD28" s="34"/>
-      <c r="BE28" s="34"/>
-      <c r="BF28" s="35"/>
-      <c r="BG28" s="33"/>
-      <c r="BH28" s="34"/>
-      <c r="BI28" s="34"/>
-      <c r="BJ28" s="35"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="34">
+        <v>1</v>
+      </c>
+      <c r="O39" s="27"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="S39" s="27"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="29"/>
+      <c r="W39" s="27"/>
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="27"/>
+      <c r="AB39" s="28"/>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="29"/>
+      <c r="AE39" s="27"/>
+      <c r="AF39" s="28"/>
+      <c r="AG39" s="28"/>
+      <c r="AH39" s="29"/>
+      <c r="AI39" s="27"/>
+      <c r="AJ39" s="28"/>
+      <c r="AK39" s="28"/>
+      <c r="AL39" s="29"/>
+      <c r="AM39" s="27"/>
+      <c r="AN39" s="28"/>
+      <c r="AO39" s="28"/>
+      <c r="AP39" s="29"/>
+      <c r="AQ39" s="27"/>
+      <c r="AR39" s="28"/>
+      <c r="AS39" s="28"/>
+      <c r="AT39" s="29"/>
+      <c r="AU39" s="27"/>
+      <c r="AV39" s="28"/>
+      <c r="AW39" s="28"/>
+      <c r="AX39" s="29"/>
+      <c r="AY39" s="27"/>
+      <c r="AZ39" s="28"/>
+      <c r="BA39" s="28"/>
+      <c r="BB39" s="29"/>
+      <c r="BC39" s="27"/>
+      <c r="BD39" s="28"/>
+      <c r="BE39" s="28"/>
+      <c r="BF39" s="29"/>
+      <c r="BG39" s="27"/>
+      <c r="BH39" s="28"/>
+      <c r="BI39" s="28"/>
+      <c r="BJ39" s="29"/>
+    </row>
+    <row r="40" spans="1:62" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="61"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="31"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="33"/>
+      <c r="O40" s="31"/>
+      <c r="P40" s="32"/>
+      <c r="Q40" s="32"/>
+      <c r="R40" s="33"/>
+      <c r="S40" s="31"/>
+      <c r="T40" s="32"/>
+      <c r="U40" s="32"/>
+      <c r="V40" s="33"/>
+      <c r="W40" s="31"/>
+      <c r="X40" s="32"/>
+      <c r="Y40" s="32"/>
+      <c r="Z40" s="33"/>
+      <c r="AA40" s="31"/>
+      <c r="AB40" s="32"/>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="33"/>
+      <c r="AE40" s="31"/>
+      <c r="AF40" s="32"/>
+      <c r="AG40" s="32"/>
+      <c r="AH40" s="33"/>
+      <c r="AI40" s="31"/>
+      <c r="AJ40" s="32"/>
+      <c r="AK40" s="32"/>
+      <c r="AL40" s="33"/>
+      <c r="AM40" s="31"/>
+      <c r="AN40" s="32"/>
+      <c r="AO40" s="32"/>
+      <c r="AP40" s="33"/>
+      <c r="AQ40" s="31"/>
+      <c r="AR40" s="32"/>
+      <c r="AS40" s="32"/>
+      <c r="AT40" s="33"/>
+      <c r="AU40" s="31"/>
+      <c r="AV40" s="32"/>
+      <c r="AW40" s="32"/>
+      <c r="AX40" s="33"/>
+      <c r="AY40" s="31"/>
+      <c r="AZ40" s="32"/>
+      <c r="BA40" s="32"/>
+      <c r="BB40" s="33"/>
+      <c r="BC40" s="31"/>
+      <c r="BD40" s="32"/>
+      <c r="BE40" s="32"/>
+      <c r="BF40" s="33"/>
+      <c r="BG40" s="31"/>
+      <c r="BH40" s="32"/>
+      <c r="BI40" s="32"/>
+      <c r="BJ40" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="B27:B28"/>
+  <mergeCells count="47">
+    <mergeCell ref="A7:A30"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D19:E22"/>
+    <mergeCell ref="D23:E26"/>
+    <mergeCell ref="D27:E30"/>
+    <mergeCell ref="BG1:BJ1"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:E18"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:E14"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="AQ1:AT1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="AY1:BB1"/>
+    <mergeCell ref="BC1:BF1"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="AE1:AH1"/>
     <mergeCell ref="W1:Z1"/>
     <mergeCell ref="AA1:AD1"/>
@@ -2593,37 +3387,12 @@
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="D3:E6"/>
-    <mergeCell ref="D23:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:E28"/>
-    <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="BC1:BF1"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="D35:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:E40"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:E34"/>
     <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:E22"/>
-    <mergeCell ref="A7:A18"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="BG1:BJ1"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:E18"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:E14"/>
-    <mergeCell ref="B19:B22"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>